<commit_message>
Working version - fixed format class generation
</commit_message>
<xml_diff>
--- a/file-parser-generator-utility/config/Field_Mapping.xlsx
+++ b/file-parser-generator-utility/config/Field_Mapping.xlsx
@@ -107,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="101">
   <si>
     <t>Header</t>
   </si>
@@ -328,15 +328,6 @@
     <t>END</t>
   </si>
   <si>
-    <t>'*'</t>
-  </si>
-  <si>
-    <t>' '</t>
-  </si>
-  <si>
-    <t>ddMMyyyy</t>
-  </si>
-  <si>
     <t>joiningDate</t>
   </si>
   <si>
@@ -361,9 +352,6 @@
     <t>salary</t>
   </si>
   <si>
-    <t>###.##</t>
-  </si>
-  <si>
     <t>In case of number or decimal  value, ask whether number should be rounded to x digits</t>
   </si>
   <si>
@@ -410,6 +398,18 @@
   </si>
   <si>
     <t>float</t>
+  </si>
+  <si>
+    <t>ddMMMyyyy</t>
+  </si>
+  <si>
+    <t>###.###</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>*</t>
   </si>
 </sst>
 </file>
@@ -890,7 +890,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -909,13 +911,13 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>1</v>
@@ -933,21 +935,21 @@
         <v>5</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -966,7 +968,7 @@
         <v>24</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>73</v>
+        <v>100</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -977,7 +979,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>19</v>
@@ -997,7 +999,7 @@
         <v>24</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>74</v>
+        <v>99</v>
       </c>
       <c r="I3" t="s">
         <v>8</v>
@@ -1005,7 +1007,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>20</v>
@@ -1025,7 +1027,7 @@
         <v>24</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>74</v>
+        <v>99</v>
       </c>
       <c r="I4" t="s">
         <v>8</v>
@@ -1033,10 +1035,10 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C5" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1052,17 +1054,19 @@
       <c r="F5" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="12"/>
+      <c r="G5" s="12" t="s">
+        <v>99</v>
+      </c>
       <c r="I5" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C6" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1073,13 +1077,14 @@
         <v>28</v>
       </c>
       <c r="E6">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F6" t="s">
         <v>24</v>
       </c>
+      <c r="G6" s="12"/>
       <c r="H6" t="s">
-        <v>75</v>
+        <v>97</v>
       </c>
       <c r="I6" t="s">
         <v>12</v>
@@ -1090,10 +1095,10 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C7" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1101,7 +1106,7 @@
       </c>
       <c r="D7" s="13">
         <f t="shared" si="1"/>
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E7">
         <v>8</v>
@@ -1109,8 +1114,11 @@
       <c r="F7" t="s">
         <v>25</v>
       </c>
+      <c r="G7" s="12" t="s">
+        <v>99</v>
+      </c>
       <c r="H7" s="15" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="I7" t="s">
         <v>15</v>
@@ -1121,7 +1129,7 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>18</v>
@@ -1132,7 +1140,7 @@
       </c>
       <c r="D8" s="13">
         <f t="shared" si="1"/>
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E8">
         <v>22</v>
@@ -1141,7 +1149,7 @@
         <v>24</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>74</v>
+        <v>99</v>
       </c>
       <c r="I8" t="s">
         <v>8</v>
@@ -1149,7 +1157,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>7</v>
@@ -1160,7 +1168,7 @@
       </c>
       <c r="D9" s="13">
         <f t="shared" si="1"/>
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E9">
         <v>5</v>
@@ -1169,7 +1177,7 @@
         <v>24</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>73</v>
+        <v>100</v>
       </c>
       <c r="I9" t="s">
         <v>8</v>
@@ -1179,7 +1187,7 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="2">
+  <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I9">
       <formula1>Datatypes</formula1>
     </dataValidation>
@@ -1203,7 +1211,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -1211,27 +1219,27 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
@@ -1292,12 +1300,12 @@
       </c>
       <c r="H1" s="12"/>
       <c r="I1" s="14" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>30</v>
@@ -1316,7 +1324,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>31</v>
@@ -1335,7 +1343,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>32</v>
@@ -1354,7 +1362,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>33</v>
@@ -1366,7 +1374,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>34</v>
@@ -1385,7 +1393,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>35</v>
@@ -1403,7 +1411,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>36</v>

</xml_diff>